<commit_message>
Lab 29 Errors Fixed, additional edema runthrough added.
</commit_message>
<xml_diff>
--- a/29_aortic_regurgitation/29_aortic_regurgitation_data.xlsx
+++ b/29_aortic_regurgitation/29_aortic_regurgitation_data.xlsx
@@ -16,9 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
-  <si>
-    <t>.12mm^2 valve closed</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="17">
+  <si>
+    <t>.12mm^2, 1 week</t>
   </si>
   <si>
     <t>Time</t>
@@ -60,7 +60,13 @@
     <t>Excess Lung H2O(mL)</t>
   </si>
   <si>
-    <t>.14mm^2 valve closed</t>
+    <t>.14mm^2, 1 week</t>
+  </si>
+  <si>
+    <t>.18mm^2, 10 days</t>
+  </si>
+  <si>
+    <t>10 Days</t>
   </si>
 </sst>
 </file>
@@ -487,23 +493,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:I12"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1">
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="30.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -528,8 +537,20 @@
       <c r="I2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="75.75" thickBot="1">
+      <c r="K2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="75.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -554,52 +575,88 @@
       <c r="I3" s="4">
         <v>4492</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="75.75" thickBot="1">
+      <c r="K3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="4">
+        <v>5361</v>
+      </c>
+      <c r="M3" s="4">
+        <v>4018</v>
+      </c>
+      <c r="N3" s="4">
+        <v>4290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="75.75" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="4">
-        <v>12.9</v>
+        <v>13</v>
       </c>
       <c r="C4" s="4">
         <v>15</v>
       </c>
       <c r="D4" s="4">
-        <v>15.3</v>
+        <v>15</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="7">
-        <v>12.9</v>
+        <v>13</v>
       </c>
       <c r="H4" s="7">
         <v>16</v>
       </c>
       <c r="I4" s="7">
-        <v>16.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="75.75" thickBot="1">
+        <v>17</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="4">
+        <v>13</v>
+      </c>
+      <c r="M4" s="4">
+        <v>20</v>
+      </c>
+      <c r="N4" s="4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="75.75" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="4">
-        <v>8.8000000000000007</v>
+        <v>9</v>
       </c>
       <c r="C5" s="4">
-        <v>12.6</v>
+        <v>13</v>
       </c>
       <c r="D5" s="4">
-        <v>13.2</v>
+        <v>13</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" ht="75.75" thickBot="1">
+      <c r="K5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" s="4">
+        <v>9</v>
+      </c>
+      <c r="M5" s="4">
+        <v>18</v>
+      </c>
+      <c r="N5" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="75.75" thickBot="1">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -616,16 +673,28 @@
         <v>7</v>
       </c>
       <c r="G6" s="4">
-        <v>8.8000000000000007</v>
+        <v>9</v>
       </c>
       <c r="H6" s="4">
         <v>14</v>
       </c>
       <c r="I6" s="4">
-        <v>14.9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="75.75" thickBot="1">
+        <v>15</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="4">
+        <v>5.7</v>
+      </c>
+      <c r="M6" s="4">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="N6" s="4">
+        <v>25.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="75.75" thickBot="1">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -636,7 +705,7 @@
         <v>9.5</v>
       </c>
       <c r="D7" s="4">
-        <v>10.199999999999999</v>
+        <v>10.3</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>8</v>
@@ -650,8 +719,20 @@
       <c r="I7" s="4">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="75.75" thickBot="1">
+      <c r="K7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="M7" s="4">
+        <v>16.3</v>
+      </c>
+      <c r="N7" s="4">
+        <v>24.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="75.75" thickBot="1">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -676,8 +757,20 @@
       <c r="I8" s="4">
         <v>12.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="45.75" thickBot="1">
+      <c r="K8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="4">
+        <v>28</v>
+      </c>
+      <c r="M8" s="4">
+        <v>28</v>
+      </c>
+      <c r="N8" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="45.75" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -702,8 +795,20 @@
       <c r="I9" s="4">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="45.75" thickBot="1">
+      <c r="K9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="4">
+        <v>91</v>
+      </c>
+      <c r="M9" s="4">
+        <v>87</v>
+      </c>
+      <c r="N9" s="4">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="45.75" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -714,7 +819,7 @@
         <v>5400</v>
       </c>
       <c r="D10" s="4">
-        <v>5504</v>
+        <v>5505</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>11</v>
@@ -728,8 +833,20 @@
       <c r="I10" s="4">
         <v>91</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="60.75" thickBot="1">
+      <c r="K10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="4">
+        <v>5400</v>
+      </c>
+      <c r="M10" s="4">
+        <v>5400</v>
+      </c>
+      <c r="N10" s="4">
+        <v>5955</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="60.75" thickBot="1">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -754,8 +871,20 @@
       <c r="I11" s="4">
         <v>5523</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="60.75" thickBot="1">
+      <c r="K11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="60.75" thickBot="1">
       <c r="F12" s="3" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Making Tentative Starts to Labs 29 and 30. Encountering Problems.
</commit_message>
<xml_diff>
--- a/29_aortic_regurgitation/29_aortic_regurgitation_data.xlsx
+++ b/29_aortic_regurgitation/29_aortic_regurgitation_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="22">
   <si>
     <t>.12mm^2, 1 week</t>
   </si>
@@ -69,7 +69,19 @@
     <t>14 Days</t>
   </si>
   <si>
-    <t>(2 weeks)</t>
+    <t>QCP</t>
+  </si>
+  <si>
+    <t>HumMod</t>
+  </si>
+  <si>
+    <t>14 days</t>
+  </si>
+  <si>
+    <t>Acute (10 mins)</t>
+  </si>
+  <si>
+    <t>HumMod does not allow for the aortic valve closed area to be fine tuned between .12 and .14 mm, only allowing increments of .1mmm^2 to be adjusted.</t>
   </si>
 </sst>
 </file>
@@ -91,15 +103,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -155,11 +173,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -167,6 +200,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -179,8 +218,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -476,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:N11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -488,70 +545,80 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
       <c r="F1" t="s">
         <v>13</v>
       </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
       <c r="K1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="30">
-      <c r="A2" s="3" t="s">
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>3</v>
+      <c r="M2" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="N2" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="30.75" thickBot="1">
-      <c r="A3" s="4"/>
-      <c r="B3" s="6"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="1" t="s">
+      <c r="D3" s="8"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="I3" s="11"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="9"/>
     </row>
     <row r="4" spans="1:14" ht="75.75" thickBot="1">
       <c r="A4" s="2" t="s">
@@ -566,16 +633,16 @@
       <c r="D4" s="1">
         <v>4493</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="12">
         <v>5346</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="12">
         <v>4576</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="12">
         <v>4285</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -604,16 +671,16 @@
       <c r="D5" s="1">
         <v>15</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="12">
         <v>13</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="12">
         <v>16</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="12">
         <v>16</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -642,10 +709,18 @@
       <c r="D6" s="1">
         <v>12</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+      <c r="F6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="12">
+        <v>9</v>
+      </c>
+      <c r="H6" s="12">
+        <v>14</v>
+      </c>
+      <c r="I6" s="12">
+        <v>14</v>
+      </c>
       <c r="K6" s="2" t="s">
         <v>7</v>
       </c>
@@ -672,17 +747,17 @@
       <c r="D7" s="1">
         <v>10.7</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="1">
-        <v>9</v>
-      </c>
-      <c r="H7" s="1">
-        <v>14</v>
-      </c>
-      <c r="I7" s="1">
-        <v>14</v>
+      <c r="F7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="12">
+        <v>5.6</v>
+      </c>
+      <c r="H7" s="12">
+        <v>12.9</v>
+      </c>
+      <c r="I7" s="12">
+        <v>12.5</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>8</v>
@@ -710,17 +785,17 @@
       <c r="D8" s="1">
         <v>9</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="1">
-        <v>5.6</v>
-      </c>
-      <c r="H8" s="1">
-        <v>12.9</v>
-      </c>
-      <c r="I8" s="1">
-        <v>12.5</v>
+      <c r="F8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="H8" s="12">
+        <v>11.2</v>
+      </c>
+      <c r="I8" s="12">
+        <v>10.9</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>9</v>
@@ -735,7 +810,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="75.75" thickBot="1">
+    <row r="9" spans="1:14" ht="45.75" thickBot="1">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -748,17 +823,17 @@
       <c r="D9" s="1">
         <v>26</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="H9" s="1">
-        <v>11.2</v>
-      </c>
-      <c r="I9" s="1">
-        <v>10.9</v>
+      <c r="F9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="12">
+        <v>28</v>
+      </c>
+      <c r="H9" s="12">
+        <v>28</v>
+      </c>
+      <c r="I9" s="12">
+        <v>26</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>10</v>
@@ -786,17 +861,17 @@
       <c r="D10" s="1">
         <v>94</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="1">
-        <v>28</v>
-      </c>
-      <c r="H10" s="1">
-        <v>28</v>
-      </c>
-      <c r="I10" s="1">
-        <v>26</v>
+      <c r="F10" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="12">
+        <v>91</v>
+      </c>
+      <c r="H10" s="12">
+        <v>85</v>
+      </c>
+      <c r="I10" s="12">
+        <v>94</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>11</v>
@@ -824,17 +899,17 @@
       <c r="D11" s="1">
         <v>5409</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="1">
-        <v>91</v>
-      </c>
-      <c r="H11" s="1">
-        <v>85</v>
-      </c>
-      <c r="I11" s="1">
-        <v>94</v>
+      <c r="F11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="12">
+        <v>5413</v>
+      </c>
+      <c r="H11" s="12">
+        <v>5406</v>
+      </c>
+      <c r="I11" s="12">
+        <v>5425</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>12</v>
@@ -849,22 +924,339 @@
         <v>5903</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="45.75" thickBot="1">
-      <c r="F12" s="2" t="s">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="32.25" customHeight="1" thickBot="1">
+      <c r="A18" s="6"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="8"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="11"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="9"/>
+    </row>
+    <row r="19" spans="1:14" ht="75.75" thickBot="1">
+      <c r="A19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1">
+        <v>5468</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="F19" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="1">
+        <v>5468</v>
+      </c>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="K19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L19" s="1">
+        <v>5468</v>
+      </c>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+    </row>
+    <row r="20" spans="1:14" ht="75.75" thickBot="1">
+      <c r="A20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="1">
+        <v>13.3</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="F20" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="1">
+        <v>13.3</v>
+      </c>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="K20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L20" s="1">
+        <v>13.3</v>
+      </c>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+    </row>
+    <row r="21" spans="1:14" ht="75.75" thickBot="1">
+      <c r="A21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="F21" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="K21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L21" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+    </row>
+    <row r="22" spans="1:14" ht="75.75" thickBot="1">
+      <c r="A22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="1">
+        <v>6.2</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="F22" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="1">
+        <v>6.2</v>
+      </c>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="K22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L22" s="1">
+        <v>6.2</v>
+      </c>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+    </row>
+    <row r="23" spans="1:14" ht="75.75" thickBot="1">
+      <c r="A23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="F23" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="K23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L23" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+    </row>
+    <row r="24" spans="1:14" ht="45.75" thickBot="1">
+      <c r="A24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="1">
+        <v>28</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="F24" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="1">
+        <v>28</v>
+      </c>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="K24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L24" s="1">
+        <v>28</v>
+      </c>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+    </row>
+    <row r="25" spans="1:14" ht="45.75" thickBot="1">
+      <c r="A25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="1">
+        <v>93</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="F25" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="1">
+        <v>93</v>
+      </c>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="K25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L25" s="1">
+        <v>93</v>
+      </c>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+    </row>
+    <row r="26" spans="1:14" ht="45.75" thickBot="1">
+      <c r="A26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="1">
-        <v>5413</v>
-      </c>
-      <c r="H12" s="1">
-        <v>5406</v>
-      </c>
-      <c r="I12" s="1">
-        <v>5425</v>
-      </c>
+      <c r="B26" s="1">
+        <v>5421</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="F26" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="1">
+        <v>5421</v>
+      </c>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="K26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L26" s="1">
+        <v>5421</v>
+      </c>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="23">
+    <mergeCell ref="A28:N29"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="C17:C18"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
@@ -874,10 +1266,6 @@
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="I2:I3"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Committing Changes to Lab 29 Notes, Moving On.
</commit_message>
<xml_diff>
--- a/29_aortic_regurgitation/29_aortic_regurgitation_data.xlsx
+++ b/29_aortic_regurgitation/29_aortic_regurgitation_data.xlsx
@@ -81,7 +81,7 @@
     <t>Acute (10 mins)</t>
   </si>
   <si>
-    <t>HumMod does not allow for the aortic valve closed area to be fine tuned between .12 and .14 mm, only allowing increments of .1mmm^2 to be adjusted.</t>
+    <t>HumMod does not allow for the aortic valve closed area to be fine tuned between .12 and .14 mm, only allowing increments of .1mmm^2 to be adjusted. Until this issue is fixed, no further work can be done.</t>
   </si>
 </sst>
 </file>
@@ -206,38 +206,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -536,7 +536,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A28" sqref="A28:N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -565,60 +565,60 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="30.75" thickBot="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12" t="s">
+      <c r="D3" s="10"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="11"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
+      <c r="I3" s="15"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="11"/>
     </row>
     <row r="4" spans="1:14" ht="75.75" thickBot="1">
       <c r="A4" s="2" t="s">
@@ -633,16 +633,16 @@
       <c r="D4" s="1">
         <v>4493</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="5">
         <v>5346</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="5">
         <v>4576</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="5">
         <v>4285</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -671,16 +671,16 @@
       <c r="D5" s="1">
         <v>15</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="5">
         <v>13</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="5">
         <v>16</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="5">
         <v>16</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -709,16 +709,16 @@
       <c r="D6" s="1">
         <v>12</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="5">
         <v>9</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="5">
         <v>14</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="5">
         <v>14</v>
       </c>
       <c r="K6" s="2" t="s">
@@ -747,16 +747,16 @@
       <c r="D7" s="1">
         <v>10.7</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="5">
         <v>5.6</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="5">
         <v>12.9</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="5">
         <v>12.5</v>
       </c>
       <c r="K7" s="2" t="s">
@@ -785,16 +785,16 @@
       <c r="D8" s="1">
         <v>9</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="5">
         <v>3.5</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="5">
         <v>11.2</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="5">
         <v>10.9</v>
       </c>
       <c r="K8" s="2" t="s">
@@ -823,16 +823,16 @@
       <c r="D9" s="1">
         <v>26</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="5">
         <v>28</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="5">
         <v>28</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="5">
         <v>26</v>
       </c>
       <c r="K9" s="2" t="s">
@@ -861,16 +861,16 @@
       <c r="D10" s="1">
         <v>94</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="5">
         <v>91</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="5">
         <v>85</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="5">
         <v>94</v>
       </c>
       <c r="K10" s="2" t="s">
@@ -899,16 +899,16 @@
       <c r="D11" s="1">
         <v>5409</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="5">
         <v>5413</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="5">
         <v>5406</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="5">
         <v>5425</v>
       </c>
       <c r="K11" s="2" t="s">
@@ -948,56 +948,56 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H17" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="I17" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="K17" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="L17" s="7" t="s">
+      <c r="L17" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="M17" s="7" t="s">
+      <c r="M17" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="N17" s="7" t="s">
+      <c r="N17" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="32.25" customHeight="1" thickBot="1">
-      <c r="A18" s="6"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="8"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="11"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="9"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="10"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="15"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="11"/>
     </row>
     <row r="19" spans="1:14" ht="75.75" thickBot="1">
       <c r="A19" s="3" t="s">
@@ -1008,14 +1008,14 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="6" t="s">
         <v>5</v>
       </c>
       <c r="G19" s="1">
         <v>5468</v>
       </c>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
       <c r="K19" s="3" t="s">
         <v>5</v>
       </c>
@@ -1034,14 +1034,14 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G20" s="1">
         <v>13.3</v>
       </c>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
       <c r="K20" s="3" t="s">
         <v>6</v>
       </c>
@@ -1060,14 +1060,14 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="F21" s="13" t="s">
+      <c r="F21" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G21" s="1">
         <v>9.1999999999999993</v>
       </c>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
       <c r="K21" s="3" t="s">
         <v>7</v>
       </c>
@@ -1086,14 +1086,14 @@
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="F22" s="13" t="s">
+      <c r="F22" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G22" s="1">
         <v>6.2</v>
       </c>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
       <c r="K22" s="3" t="s">
         <v>8</v>
       </c>
@@ -1112,14 +1112,14 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="F23" s="13" t="s">
+      <c r="F23" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G23" s="1">
         <v>5.2</v>
       </c>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
       <c r="K23" s="3" t="s">
         <v>9</v>
       </c>
@@ -1138,14 +1138,14 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G24" s="1">
         <v>28</v>
       </c>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
       <c r="K24" s="3" t="s">
         <v>10</v>
       </c>
@@ -1164,14 +1164,14 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="F25" s="13" t="s">
+      <c r="F25" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G25" s="1">
         <v>93</v>
       </c>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
       <c r="K25" s="3" t="s">
         <v>11</v>
       </c>
@@ -1190,14 +1190,14 @@
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-      <c r="F26" s="13" t="s">
+      <c r="F26" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G26" s="1">
         <v>5421</v>
       </c>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
       <c r="K26" s="3" t="s">
         <v>12</v>
       </c>
@@ -1208,41 +1208,48 @@
       <c r="N26" s="1"/>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="I2:I3"/>
     <mergeCell ref="A28:N29"/>
     <mergeCell ref="L17:L18"/>
     <mergeCell ref="M17:M18"/>
@@ -1259,13 +1266,6 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="I2:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>